<commit_message>
30-05-2024: Projeto quase concluído, faltando últimos ajustes
</commit_message>
<xml_diff>
--- a/Bases de Dados/Emails.xlsx
+++ b/Bases de Dados/Emails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\ProjetoAutomacaoDeIndicadoresEnvioOnePage\Bases de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8FD3A6-C8F9-4761-85FB-0E341CEA896F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915D3B55-F595-4BEB-A5E8-FCD8377F4B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE9D8D8A-F7B1-481B-B9DF-10FF6CFE8B3E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EE9D8D8A-F7B1-481B-B9DF-10FF6CFE8B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>Gerente</t>
   </si>
   <si>
-    <t>E-mail</t>
-  </si>
-  <si>
     <t>Iguatemi Esplanada</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>carlosrodriguesjfprojects+diretoria@gmail.com</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -627,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D81E77-7AEF-4DB7-8688-DEDDD091CFFB}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,7 +640,7 @@
     <col min="3" max="3" width="43.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -648,295 +648,295 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C14" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>